<commit_message>
graph with tokens fixed
</commit_message>
<xml_diff>
--- a/graphwithtokens.xlsx
+++ b/graphwithtokens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fe56d8f8de21353/Documents/Deep Learning/playing_with_clip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="8_{BB129E25-17D0-402B-B27D-502B85FAE7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4C04495-66CA-445E-89F2-B5654FE452EF}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="8_{BB129E25-17D0-402B-B27D-502B85FAE7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5520C3F-E5D1-4501-93D5-0796E71C69B0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="121">
   <si>
     <t>Token Info</t>
   </si>
@@ -103,9 +103,6 @@
     <t>5: ☺☺</t>
   </si>
   <si>
-    <t xml:space="preserve"># </t>
-  </si>
-  <si>
     <t>DTD</t>
   </si>
   <si>
@@ -383,13 +380,19 @@
   </si>
   <si>
     <t>"A picture of the flower"</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Token </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,12 +425,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Aptos Mono"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="6"/>
@@ -549,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -591,54 +588,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,7 +783,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>924983</xdr:colOff>
+      <xdr:colOff>924982</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>42384</xdr:rowOff>
     </xdr:to>
@@ -1426,13 +1415,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0ABFB1-D72B-4648-9A55-4C6A86D4D6E0}">
   <dimension ref="A1:AA41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
@@ -1465,47 +1454,47 @@
       <c r="Z1" s="7"/>
     </row>
     <row r="2" spans="1:27" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
       <c r="G2" s="7"/>
       <c r="X2" s="7"/>
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
     </row>
     <row r="3" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="7"/>
       <c r="X3" s="7"/>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="1:27" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="38" t="s">
+      <c r="D4" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="E4" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="F4" s="34" t="s">
         <v>29</v>
-      </c>
-      <c r="F4" s="39" t="s">
-        <v>30</v>
       </c>
       <c r="G4" s="7"/>
       <c r="O4" s="13"/>
@@ -1518,13 +1507,15 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:27" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="38"/>
+    <row r="5" spans="1:27" ht="10.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="33"/>
       <c r="G5" s="7"/>
       <c r="O5" s="13"/>
       <c r="P5" s="15"/>
@@ -1537,12 +1528,12 @@
       <c r="Z5" s="7"/>
     </row>
     <row r="6" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="25"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="39"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="7"/>
       <c r="O6" s="16"/>
       <c r="P6" s="15"/>
@@ -1555,23 +1546,23 @@
       <c r="Z6" s="7"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A7" s="24">
+      <c r="A7" s="22">
         <v>0</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>95</v>
+      <c r="B7" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>94</v>
       </c>
       <c r="G7" s="7"/>
       <c r="O7" s="17"/>
@@ -1585,23 +1576,23 @@
       <c r="Z7" s="7"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A8" s="24">
+      <c r="A8" s="22">
         <v>1</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>96</v>
+      <c r="B8" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="G8" s="7"/>
       <c r="O8" s="17"/>
@@ -1615,23 +1606,23 @@
       <c r="Z8" s="7"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A9" s="24">
+      <c r="A9" s="22">
         <v>2</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>97</v>
+      <c r="B9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="G9" s="7"/>
       <c r="O9" s="17"/>
@@ -1645,23 +1636,23 @@
       <c r="Z9" s="7"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A10" s="24">
+      <c r="A10" s="22">
         <v>3</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>98</v>
+      <c r="B10" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="G10" s="7"/>
       <c r="O10" s="17"/>
@@ -1675,23 +1666,23 @@
       <c r="Z10" s="7"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A11" s="24">
+      <c r="A11" s="22">
         <v>4</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>99</v>
+      <c r="B11" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>98</v>
       </c>
       <c r="G11" s="7"/>
       <c r="O11" s="17"/>
@@ -1705,23 +1696,23 @@
       <c r="Z11" s="7"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A12" s="24">
+      <c r="A12" s="22">
         <v>5</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>100</v>
+      <c r="B12" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>99</v>
       </c>
       <c r="G12" s="7"/>
       <c r="O12" s="17"/>
@@ -1735,23 +1726,23 @@
       <c r="Z12" s="7"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A13" s="24">
+      <c r="A13" s="22">
         <v>6</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>101</v>
+      <c r="B13" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>100</v>
       </c>
       <c r="G13" s="7"/>
       <c r="O13" s="17"/>
@@ -1765,23 +1756,23 @@
       <c r="Z13" s="7"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A14" s="24">
+      <c r="A14" s="22">
         <v>7</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>102</v>
+      <c r="B14" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>101</v>
       </c>
       <c r="G14" s="7"/>
       <c r="O14" s="17"/>
@@ -1795,23 +1786,23 @@
       <c r="Z14" s="7"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A15" s="24">
+      <c r="A15" s="22">
         <v>8</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>103</v>
+      <c r="B15" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>102</v>
       </c>
       <c r="G15" s="7"/>
       <c r="O15" s="17"/>
@@ -1826,23 +1817,23 @@
       <c r="AA15" s="12"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A16" s="24">
+      <c r="A16" s="22">
         <v>9</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>104</v>
+      <c r="B16" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>103</v>
       </c>
       <c r="G16" s="7"/>
       <c r="O16" s="17"/>
@@ -1857,23 +1848,23 @@
       <c r="AA16" s="12"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A17" s="24">
+      <c r="A17" s="22">
         <v>10</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>105</v>
+      <c r="B17" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>104</v>
       </c>
       <c r="G17" s="7"/>
       <c r="O17" s="17"/>
@@ -1888,23 +1879,23 @@
       <c r="AA17" s="12"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A18" s="24">
+      <c r="A18" s="22">
         <v>11</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>106</v>
+      <c r="B18" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>105</v>
       </c>
       <c r="G18" s="7"/>
       <c r="O18" s="17"/>
@@ -1919,23 +1910,23 @@
       <c r="AA18" s="12"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A19" s="24">
+      <c r="A19" s="22">
         <v>12</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>107</v>
+      <c r="B19" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>106</v>
       </c>
       <c r="G19" s="7"/>
       <c r="O19" s="17"/>
@@ -1950,23 +1941,23 @@
       <c r="AA19" s="12"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A20" s="24">
+      <c r="A20" s="22">
         <v>13</v>
       </c>
-      <c r="B20" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>108</v>
+      <c r="B20" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>107</v>
       </c>
       <c r="G20" s="7"/>
       <c r="O20" s="17"/>
@@ -1981,23 +1972,23 @@
       <c r="AA20" s="12"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A21" s="24">
+      <c r="A21" s="22">
         <v>14</v>
       </c>
-      <c r="B21" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>109</v>
+      <c r="B21" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>108</v>
       </c>
       <c r="G21" s="7"/>
       <c r="O21" s="17"/>
@@ -2012,23 +2003,23 @@
       <c r="AA21" s="12"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A22" s="24">
+      <c r="A22" s="22">
         <v>15</v>
       </c>
-      <c r="B22" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>110</v>
+      <c r="B22" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>109</v>
       </c>
       <c r="G22" s="7"/>
       <c r="O22" s="17"/>
@@ -2043,12 +2034,12 @@
       <c r="AA22" s="12"/>
     </row>
     <row r="23" spans="1:27" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="7"/>
       <c r="Q23" s="17"/>
       <c r="R23" s="17"/>
@@ -2180,85 +2171,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="30"/>
-      <c r="B1" s="31" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="D1" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="E1" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="31" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="27">
+        <v>1</v>
+      </c>
+      <c r="C2" s="28">
+        <v>0.748</v>
+      </c>
+      <c r="D2" s="29">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="E2" s="30">
+        <v>0.63900000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B3" s="28">
+        <v>0.748</v>
+      </c>
+      <c r="C3" s="27">
         <v>1</v>
       </c>
-      <c r="C2" s="33">
-        <v>0.748</v>
-      </c>
-      <c r="D2" s="34">
+      <c r="D3" s="30">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="E3" s="31">
+        <v>0.58399999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="29">
         <v>0.70799999999999996</v>
       </c>
-      <c r="E2" s="35">
+      <c r="C4" s="30">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="D4" s="27">
+        <v>1</v>
+      </c>
+      <c r="E4" s="32">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="30">
         <v>0.63900000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="33">
-        <v>0.748</v>
-      </c>
-      <c r="C3" s="32">
-        <v>1</v>
-      </c>
-      <c r="D3" s="35">
-        <v>0.65800000000000003</v>
-      </c>
-      <c r="E3" s="36">
+      <c r="C5" s="31">
         <v>0.58399999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="34">
-        <v>0.70799999999999996</v>
-      </c>
-      <c r="C4" s="35">
-        <v>0.65800000000000003</v>
-      </c>
-      <c r="D4" s="32">
-        <v>1</v>
-      </c>
-      <c r="E4" s="37">
+      <c r="D5" s="32">
         <v>0.89500000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" s="35">
-        <v>0.63900000000000001</v>
-      </c>
-      <c r="C5" s="36">
-        <v>0.58399999999999996</v>
-      </c>
-      <c r="D5" s="37">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="E5" s="32">
+      <c r="E5" s="27">
         <v>1</v>
       </c>
     </row>
@@ -2277,101 +2268,101 @@
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="D8" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="E8" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>119</v>
-      </c>
       <c r="H8" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="25">
+        <v>1</v>
+      </c>
+      <c r="C9" s="25">
+        <v>0.748</v>
+      </c>
+      <c r="D9" s="25">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="E9" s="25">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B10" s="25">
+        <v>0.748</v>
+      </c>
+      <c r="C10" s="25">
         <v>1</v>
       </c>
-      <c r="C9" s="29">
-        <v>0.748</v>
-      </c>
-      <c r="D9" s="29">
+      <c r="D10" s="25">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="E10" s="25">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="25">
         <v>0.70799999999999996</v>
       </c>
-      <c r="E9" s="29">
+      <c r="C11" s="25">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="D11" s="25">
+        <v>1</v>
+      </c>
+      <c r="E11" s="25">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="25">
         <v>0.63900000000000001</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" s="29">
-        <v>0.748</v>
-      </c>
-      <c r="C10" s="29">
+      <c r="C12" s="25">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="D12" s="25">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="E12" s="25">
         <v>1</v>
       </c>
-      <c r="D10" s="29">
-        <v>0.65800000000000003</v>
-      </c>
-      <c r="E10" s="29">
-        <v>0.58399999999999996</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="29">
-        <v>0.70799999999999996</v>
-      </c>
-      <c r="C11" s="29">
-        <v>0.65800000000000003</v>
-      </c>
-      <c r="D11" s="29">
-        <v>1</v>
-      </c>
-      <c r="E11" s="29">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="H11" s="12" t="s">
+      <c r="H12" s="12" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="B12" s="29">
-        <v>0.63900000000000001</v>
-      </c>
-      <c r="C12" s="29">
-        <v>0.58399999999999996</v>
-      </c>
-      <c r="D12" s="29">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="E12" s="29">
-        <v>1</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>